<commit_message>
accident stats, cost effectivness, emissions cost, transit time
</commit_message>
<xml_diff>
--- a/data/accident_statistics.xlsx
+++ b/data/accident_statistics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eurocontrol.sharepoint.com/sites/ECTL-Business_Cases/Shared Documents/Standard_Inputs/1. NEW_2022/Values/Accident incident statistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="481" documentId="11_1907E190FF127590693BE2FD12BAD134020208C0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7319B616-5AB1-42A5-8C0B-54DD7523D4D6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DB02C2-EE44-440F-9D0F-5479843075B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cat" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,6 @@
     <sheet name="specialops" sheetId="3" r:id="rId3"/>
     <sheet name="noncom" sheetId="4" r:id="rId4"/>
     <sheet name="atm" sheetId="9" r:id="rId5"/>
-    <sheet name="rotor" sheetId="6" r:id="rId6"/>
-    <sheet name="specialopsrotor" sheetId="7" r:id="rId7"/>
-    <sheet name="noncomrotor" sheetId="8" r:id="rId8"/>
-    <sheet name="allrotor" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -425,7 +421,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757BA636-DE0F-4DDB-9F81-54C2BEFACD54}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -755,7 +751,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +946,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F9"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8A91C0-2A9D-4FBE-880C-B06027CA5DF6}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,827 +1313,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77850345-220F-4521-A954-2CB563FF56D3}">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>24</v>
-      </c>
-      <c r="D2">
-        <v>16</v>
-      </c>
-      <c r="E2">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2020</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2019</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2018</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2017</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2016</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>21</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2015</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2014</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F7C471-8A68-4E31-A7DD-96F8936B9471}">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2020</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2019</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2018</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2017</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2016</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2015</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2014</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BB3A35-77CD-4B10-9B6F-5C3F5F9AB0A3}">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>17</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2020</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2019</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>35</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2018</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>24</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2017</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2016</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>33</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>11</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2015</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2014</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>16</v>
-      </c>
-      <c r="F9">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8991DB06-382F-47C1-A70A-47EAF589D769}">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
-      </c>
-      <c r="B2">
-        <f>SUM(rotor!B2,specialopsrotor!B2,noncomrotor!B2)</f>
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <f>SUM(rotor!C2,specialopsrotor!C2,noncomrotor!C2)</f>
-        <v>45</v>
-      </c>
-      <c r="D2">
-        <f>SUM(rotor!D2,specialopsrotor!D2,noncomrotor!D2)</f>
-        <v>24</v>
-      </c>
-      <c r="E2">
-        <f>SUM(rotor!E2,specialopsrotor!E2,noncomrotor!E2)</f>
-        <v>25</v>
-      </c>
-      <c r="F2">
-        <f>SUM(rotor!F2,specialopsrotor!F2,noncomrotor!F2)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2020</v>
-      </c>
-      <c r="B3">
-        <f>SUM(rotor!B3,specialopsrotor!B3,noncomrotor!B3)</f>
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <f>SUM(rotor!C3,specialopsrotor!C3,noncomrotor!C3)</f>
-        <v>24</v>
-      </c>
-      <c r="D3">
-        <f>SUM(rotor!D3,specialopsrotor!D3,noncomrotor!D3)</f>
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <f>SUM(rotor!E3,specialopsrotor!E3,noncomrotor!E3)</f>
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <f>SUM(rotor!F3,specialopsrotor!F3,noncomrotor!F3)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2019</v>
-      </c>
-      <c r="B4">
-        <f>SUM(rotor!B4,specialopsrotor!B4,noncomrotor!B4)</f>
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <f>SUM(rotor!C4,specialopsrotor!C4,noncomrotor!C4)</f>
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <f>SUM(rotor!D4,specialopsrotor!D4,noncomrotor!D4)</f>
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <f>SUM(rotor!E4,specialopsrotor!E4,noncomrotor!E4)</f>
-        <v>23</v>
-      </c>
-      <c r="F4">
-        <f>SUM(rotor!F4,specialopsrotor!F4,noncomrotor!F4)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2018</v>
-      </c>
-      <c r="B5">
-        <f>SUM(rotor!B5,specialopsrotor!B5,noncomrotor!B5)</f>
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <f>SUM(rotor!C5,specialopsrotor!C5,noncomrotor!C5)</f>
-        <v>43</v>
-      </c>
-      <c r="D5">
-        <f>SUM(rotor!D5,specialopsrotor!D5,noncomrotor!D5)</f>
-        <v>21</v>
-      </c>
-      <c r="E5">
-        <f>SUM(rotor!E5,specialopsrotor!E5,noncomrotor!E5)</f>
-        <v>25</v>
-      </c>
-      <c r="F5">
-        <f>SUM(rotor!F5,specialopsrotor!F5,noncomrotor!F5)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2017</v>
-      </c>
-      <c r="B6">
-        <f>SUM(rotor!B6,specialopsrotor!B6,noncomrotor!B6)</f>
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <f>SUM(rotor!C6,specialopsrotor!C6,noncomrotor!C6)</f>
-        <v>38</v>
-      </c>
-      <c r="D6">
-        <f>SUM(rotor!D6,specialopsrotor!D6,noncomrotor!D6)</f>
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <f>SUM(rotor!E6,specialopsrotor!E6,noncomrotor!E6)</f>
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <f>SUM(rotor!F6,specialopsrotor!F6,noncomrotor!F6)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2016</v>
-      </c>
-      <c r="B7">
-        <f>SUM(rotor!B7,specialopsrotor!B7,noncomrotor!B7)</f>
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <f>SUM(rotor!C7,specialopsrotor!C7,noncomrotor!C7)</f>
-        <v>51</v>
-      </c>
-      <c r="D7">
-        <f>SUM(rotor!D7,specialopsrotor!D7,noncomrotor!D7)</f>
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <f>SUM(rotor!E7,specialopsrotor!E7,noncomrotor!E7)</f>
-        <v>32</v>
-      </c>
-      <c r="F7">
-        <f>SUM(rotor!F7,specialopsrotor!F7,noncomrotor!F7)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2015</v>
-      </c>
-      <c r="B8">
-        <f>SUM(rotor!B8,specialopsrotor!B8,noncomrotor!B8)</f>
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <f>SUM(rotor!C8,specialopsrotor!C8,noncomrotor!C8)</f>
-        <v>50</v>
-      </c>
-      <c r="D8">
-        <f>SUM(rotor!D8,specialopsrotor!D8,noncomrotor!D8)</f>
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <f>SUM(rotor!E8,specialopsrotor!E8,noncomrotor!E8)</f>
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <f>SUM(rotor!F8,specialopsrotor!F8,noncomrotor!F8)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2014</v>
-      </c>
-      <c r="B9">
-        <f>SUM(rotor!B9,specialopsrotor!B9,noncomrotor!B9)</f>
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <f>SUM(rotor!C9,specialopsrotor!C9,noncomrotor!C9)</f>
-        <v>78</v>
-      </c>
-      <c r="D9">
-        <f>SUM(rotor!D9,specialopsrotor!D9,noncomrotor!D9)</f>
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <f>SUM(rotor!E9,specialopsrotor!E9,noncomrotor!E9)</f>
-        <v>22</v>
-      </c>
-      <c r="F9">
-        <f>SUM(rotor!F9,specialopsrotor!F9,noncomrotor!F9)</f>
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="841a37d2-6ac6-4cb8-8211-c8824e7b4dcd">
@@ -2146,15 +1331,6 @@
     <TaxCatchAll xmlns="c78a888a-83d8-49bb-8890-6eb97e8a3c0e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2401,6 +1577,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B72AB5AD-8548-44D3-B007-F68C0CB5074C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3FD09CC-19E0-4F63-BBCB-ACB20A1BAD2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="841a37d2-6ac6-4cb8-8211-c8824e7b4dcd"/>
@@ -2413,14 +1597,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="c78a888a-83d8-49bb-8890-6eb97e8a3c0e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B72AB5AD-8548-44D3-B007-F68C0CB5074C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>